<commit_message>
before replacing RDS with csv
</commit_message>
<xml_diff>
--- a/lists_out/allergies.xlsx
+++ b/lists_out/allergies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elsiehorne/Docs/read_codes/lists_out/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2130EB35-AFED-BD4B-B726-B4F3C2CD1D3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0C5E34AF-4B1C-3E43-BFCC-3D2757199F99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-6340" windowWidth="38400" windowHeight="21600" activeTab="2"/>
+    <workbookView xWindow="28800" yWindow="-6340" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anaphylaxis" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="11177" uniqueCount="4461">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="11228" uniqueCount="4470">
   <si>
     <t>variable</t>
   </si>
@@ -13416,12 +13416,39 @@
   </si>
   <si>
     <t>all adults so can remove</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>all yellow in, rationale is that the 'allergy' defintion is a mechanism.</t>
+  </si>
+  <si>
+    <t>exclude</t>
+  </si>
+  <si>
+    <t>include</t>
+  </si>
+  <si>
+    <t>rationale that people who react to irritants are likely to be sensitive to irritants/allergens</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>version 3</t>
+  </si>
+  <si>
+    <t>put in other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bunged up nose after stopping decongestant </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -14265,11 +14292,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14829,7 +14856,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -14846,7 +14873,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -14863,7 +14890,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -14880,7 +14907,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -14897,7 +14924,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -14914,7 +14941,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -14931,7 +14958,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
@@ -14947,8 +14974,11 @@
       <c r="E39" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -14965,7 +14995,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -14988,11 +15018,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F77"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15002,9 +15032,10 @@
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15023,8 +15054,11 @@
       <c r="F1" s="1" t="s">
         <v>4459</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>4462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -15041,7 +15075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -15058,7 +15092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
@@ -15075,7 +15109,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>90</v>
       </c>
@@ -15092,7 +15126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
@@ -15109,7 +15143,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -15126,7 +15160,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>90</v>
       </c>
@@ -15143,7 +15177,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -15160,7 +15194,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>90</v>
       </c>
@@ -15177,7 +15211,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -15194,7 +15228,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>90</v>
       </c>
@@ -15211,7 +15245,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -15228,7 +15262,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -15245,7 +15279,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -15262,7 +15296,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -16322,11 +16356,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16338,7 +16372,7 @@
     <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16358,7 +16392,7 @@
         <v>4459</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>242</v>
       </c>
@@ -16375,7 +16409,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -16392,7 +16426,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -16409,7 +16443,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>242</v>
       </c>
@@ -16426,7 +16460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>242</v>
       </c>
@@ -16443,7 +16477,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>242</v>
       </c>
@@ -16460,7 +16494,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>242</v>
       </c>
@@ -16477,7 +16511,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>242</v>
       </c>
@@ -16494,7 +16528,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -16511,7 +16545,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>242</v>
       </c>
@@ -16528,7 +16562,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>242</v>
       </c>
@@ -16545,7 +16579,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>242</v>
       </c>
@@ -16561,8 +16595,14 @@
       <c r="E13" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="2" t="s">
+        <v>4464</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>242</v>
       </c>
@@ -16577,6 +16617,9 @@
       </c>
       <c r="E14" s="2" t="s">
         <v>270</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>4464</v>
       </c>
     </row>
   </sheetData>
@@ -16585,7 +16628,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F1617"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -44098,11 +44141,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F280"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:G280"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101:XFD101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45750,7 +45793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45767,7 +45810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45784,7 +45827,7 @@
         <v>3707</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45801,7 +45844,7 @@
         <v>3710</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45818,7 +45861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45834,8 +45877,14 @@
       <c r="E101" s="3" t="s">
         <v>3713</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="3" t="s">
+        <v>4466</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>4467</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45851,8 +45900,11 @@
       <c r="E102" s="3" t="s">
         <v>3715</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="3" t="s">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45869,7 +45921,7 @@
         <v>3717</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45886,7 +45938,7 @@
         <v>3719</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45903,7 +45955,7 @@
         <v>3721</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45920,7 +45972,7 @@
         <v>3723</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45937,7 +45989,7 @@
         <v>3725</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45954,7 +46006,7 @@
         <v>3727</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45971,7 +46023,7 @@
         <v>3729</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>3505</v>
       </c>
@@ -45988,7 +46040,7 @@
         <v>3731</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>3505</v>
       </c>
@@ -46005,7 +46057,7 @@
         <v>3733</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>3505</v>
       </c>
@@ -48884,7 +48936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49453,11 +49505,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -49744,8 +49796,11 @@
       <c r="E16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>4376</v>
       </c>
@@ -49761,8 +49816,11 @@
       <c r="E17" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="2" t="s">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4376</v>
       </c>
@@ -49779,7 +49837,7 @@
         <v>4414</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4376</v>
       </c>
@@ -49796,7 +49854,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4376</v>
       </c>
@@ -49813,7 +49871,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4376</v>
       </c>
@@ -49829,8 +49887,11 @@
       <c r="E21" t="s">
         <v>4420</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4376</v>
       </c>
@@ -49846,8 +49907,11 @@
       <c r="E22" t="s">
         <v>4422</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4376</v>
       </c>
@@ -49863,8 +49927,11 @@
       <c r="E23" t="s">
         <v>4424</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4376</v>
       </c>
@@ -49880,8 +49947,11 @@
       <c r="E24" t="s">
         <v>4426</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4376</v>
       </c>
@@ -49897,8 +49967,14 @@
       <c r="E25" t="s">
         <v>4428</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>4463</v>
+      </c>
+      <c r="G25" t="s">
+        <v>4469</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4376</v>
       </c>
@@ -49914,8 +49990,11 @@
       <c r="E26" t="s">
         <v>4430</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4376</v>
       </c>
@@ -49931,8 +50010,11 @@
       <c r="E27" t="s">
         <v>4432</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>4376</v>
       </c>
@@ -49948,8 +50030,11 @@
       <c r="E28" t="s">
         <v>4434</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4376</v>
       </c>
@@ -49965,8 +50050,11 @@
       <c r="E29" t="s">
         <v>4436</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>4376</v>
       </c>
@@ -49982,8 +50070,11 @@
       <c r="E30" t="s">
         <v>4438</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4376</v>
       </c>
@@ -49999,8 +50090,11 @@
       <c r="E31" t="s">
         <v>4440</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>4376</v>
       </c>
@@ -50016,8 +50110,11 @@
       <c r="E32" t="s">
         <v>4442</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4376</v>
       </c>
@@ -50033,8 +50130,11 @@
       <c r="E33" t="s">
         <v>4444</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4376</v>
       </c>
@@ -50050,8 +50150,11 @@
       <c r="E34" t="s">
         <v>4446</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>4376</v>
       </c>
@@ -50067,8 +50170,11 @@
       <c r="E35" t="s">
         <v>4448</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4376</v>
       </c>
@@ -50084,8 +50190,11 @@
       <c r="E36" t="s">
         <v>4450</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>4376</v>
       </c>
@@ -50101,8 +50210,11 @@
       <c r="E37" t="s">
         <v>4452</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4376</v>
       </c>
@@ -50117,6 +50229,9 @@
       </c>
       <c r="E38" t="s">
         <v>4454</v>
+      </c>
+      <c r="F38" t="s">
+        <v>4461</v>
       </c>
     </row>
   </sheetData>
@@ -50125,7 +50240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -50286,11 +50401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:XFD119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50577,7 +50692,7 @@
         <v>4152</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4125</v>
       </c>
@@ -50594,7 +50709,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4125</v>
       </c>
@@ -50611,7 +50726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4125</v>
       </c>
@@ -50628,7 +50743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>4125</v>
       </c>
@@ -50645,7 +50760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50661,8 +50776,11 @@
       <c r="E21" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="2" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4125</v>
       </c>
@@ -50679,7 +50797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4125</v>
       </c>
@@ -50696,7 +50814,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4125</v>
       </c>
@@ -50713,7 +50831,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>4125</v>
       </c>
@@ -50730,7 +50848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4125</v>
       </c>
@@ -50747,7 +50865,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50763,8 +50881,11 @@
       <c r="E27" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50780,8 +50901,11 @@
       <c r="E28" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50797,8 +50921,11 @@
       <c r="E29" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50814,8 +50941,11 @@
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50831,8 +50961,11 @@
       <c r="E31" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50848,8 +50981,11 @@
       <c r="E32" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50865,8 +51001,11 @@
       <c r="E33" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50882,8 +51021,11 @@
       <c r="E34" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50899,8 +51041,11 @@
       <c r="E35" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50916,8 +51061,11 @@
       <c r="E36" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50933,8 +51081,11 @@
       <c r="E37" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50950,8 +51101,11 @@
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50967,8 +51121,11 @@
       <c r="E39" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>4125</v>
       </c>
@@ -50984,8 +51141,11 @@
       <c r="E40" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>4125</v>
       </c>
@@ -51001,8 +51161,11 @@
       <c r="E41" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>4125</v>
       </c>
@@ -51018,8 +51181,11 @@
       <c r="E42" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>4125</v>
       </c>
@@ -51035,8 +51201,11 @@
       <c r="E43" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>4125</v>
       </c>
@@ -51052,8 +51221,11 @@
       <c r="E44" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>4125</v>
       </c>
@@ -51069,8 +51241,11 @@
       <c r="E45" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="2" t="s">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4125</v>
       </c>
@@ -51087,7 +51262,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>4125</v>
       </c>
@@ -51104,7 +51279,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>4125</v>
       </c>
@@ -51307,6 +51482,9 @@
       <c r="E59" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="F59" s="2" t="s">
+        <v>4463</v>
+      </c>
       <c r="G59" s="2" t="s">
         <v>4460</v>
       </c>
@@ -51396,7 +51574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>4125</v>
       </c>
@@ -51413,7 +51591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>4125</v>
       </c>
@@ -51430,7 +51608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>4125</v>
       </c>
@@ -51447,7 +51625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>4125</v>
       </c>
@@ -51464,7 +51642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>4125</v>
       </c>
@@ -51481,7 +51659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>4125</v>
       </c>
@@ -51498,7 +51676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>4125</v>
       </c>
@@ -51515,7 +51693,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>4125</v>
       </c>
@@ -51531,8 +51709,11 @@
       <c r="E72" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="2" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>4125</v>
       </c>
@@ -51549,7 +51730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>4125</v>
       </c>
@@ -51566,7 +51747,7 @@
         <v>4267</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>4125</v>
       </c>
@@ -51583,7 +51764,7 @@
         <v>4269</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>4125</v>
       </c>
@@ -51600,7 +51781,7 @@
         <v>4271</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>4125</v>
       </c>
@@ -51617,7 +51798,7 @@
         <v>4273</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>4125</v>
       </c>
@@ -51634,7 +51815,7 @@
         <v>4275</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>4125</v>
       </c>
@@ -51651,7 +51832,7 @@
         <v>4277</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>4125</v>
       </c>

</xml_diff>